<commit_message>
The 23 of May 2024
</commit_message>
<xml_diff>
--- a/src/Components/Assets/Excels/2024_Master1_Semestre1.xlsx
+++ b/src/Components/Assets/Excels/2024_Master1_Semestre1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\webspace\tiska\src\Server\Cba\Grilles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\devspace\ttiska\src\Components\Assets\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5990"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5985"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Noms</t>
   </si>
@@ -59,15 +59,6 @@
     <t>systeme</t>
   </si>
   <si>
-    <t>c2math</t>
-  </si>
-  <si>
-    <t>u1anglais5c</t>
-  </si>
-  <si>
-    <t>u2info5c</t>
-  </si>
-  <si>
     <t>annee</t>
   </si>
   <si>
@@ -98,7 +89,28 @@
     <t>complements_valides</t>
   </si>
   <si>
-    <t>…</t>
+    <t>faculte</t>
+  </si>
+  <si>
+    <t>sciences</t>
+  </si>
+  <si>
+    <t>departement</t>
+  </si>
+  <si>
+    <t>math-info</t>
+  </si>
+  <si>
+    <t>u2c5anglais</t>
+  </si>
+  <si>
+    <t>u2c5informatique</t>
+  </si>
+  <si>
+    <t>u2c5mathematique</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -154,16 +166,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:O3" totalsRowShown="0">
-  <autoFilter ref="A1:O3"/>
-  <tableColumns count="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:Q3" totalsRowShown="0">
+  <autoFilter ref="A1:Q3"/>
+  <tableColumns count="17">
     <tableColumn id="1" name="Noms"/>
     <tableColumn id="2" name="filiere"/>
     <tableColumn id="3" name="promotion"/>
     <tableColumn id="4" name="systeme"/>
-    <tableColumn id="5" name="u1anglais5c"/>
-    <tableColumn id="6" name="u2info5c"/>
-    <tableColumn id="7" name="c2math"/>
+    <tableColumn id="5" name="u2c5anglais"/>
+    <tableColumn id="6" name="u2c5informatique"/>
+    <tableColumn id="7" name="u2c5mathematique"/>
     <tableColumn id="8" name="annee"/>
     <tableColumn id="9" name="credits"/>
     <tableColumn id="10" name="credits_valides"/>
@@ -172,6 +184,8 @@
     <tableColumn id="13" name="moyenne_ponderee"/>
     <tableColumn id="14" name="decision_jury"/>
     <tableColumn id="15" name="complements_valides"/>
+    <tableColumn id="16" name="faculte"/>
+    <tableColumn id="17" name="departement"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -440,20 +454,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.6328125" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
+    <col min="13" max="13" width="24.42578125" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+    <col min="15" max="15" width="27.140625" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,40 +492,46 @@
         <v>10</v>
       </c>
       <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -531,23 +562,29 @@
       <c r="J2">
         <v>60</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" t="s">
         <v>22</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -578,26 +615,33 @@
       <c r="J3">
         <v>60</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
       </c>
       <c r="M3">
         <v>14</v>
       </c>
       <c r="N3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" t="s">
         <v>22</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>